<commit_message>
home page work will begin
</commit_message>
<xml_diff>
--- a/server/Expenses_details.xlsx
+++ b/server/Expenses_details.xlsx
@@ -64,9 +64,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -421,8 +420,8 @@
       <c r="B2" t="str">
         <v>rent</v>
       </c>
-      <c r="C2" s="1">
-        <v>46023.00011574074</v>
+      <c r="C2" t="str">
+        <v>2025-12-31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
project is ready to deploy
</commit_message>
<xml_diff>
--- a/server/Expenses_details.xlsx
+++ b/server/Expenses_details.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -415,18 +415,73 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>12000</v>
+        <v>360</v>
       </c>
       <c r="B2" t="str">
-        <v>rent</v>
+        <v>hair cut</v>
       </c>
       <c r="C2" t="str">
-        <v>2025-12-31</v>
+        <v>20/12/2026</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3">
+        <v>390</v>
+      </c>
+      <c r="B3" t="str">
+        <v>cloth</v>
+      </c>
+      <c r="C3" t="str">
+        <v>02/11/2026</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4">
+        <v>500</v>
+      </c>
+      <c r="B4" t="str">
+        <v>food</v>
+      </c>
+      <c r="C4" t="str">
+        <v>01/11/2026</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5">
+        <v>7500</v>
+      </c>
+      <c r="B5" t="str">
+        <v>shopping</v>
+      </c>
+      <c r="C5" t="str">
+        <v>28/01/2026</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6">
+        <v>360</v>
+      </c>
+      <c r="B6" t="str">
+        <v>cloth</v>
+      </c>
+      <c r="C6" t="str">
+        <v>20/01/2026</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7">
+        <v>50</v>
+      </c>
+      <c r="B7" t="str">
+        <v>food</v>
+      </c>
+      <c r="C7" t="str">
+        <v>01/01/2026</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C7"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>